<commit_message>
Fix: unify emissions chart colors and stacking order (BAU, NCNC, Interactive) using theme-based config; update all data files with latest interactive datasets
</commit_message>
<xml_diff>
--- a/data/Fable_46_Agricultural.xlsx
+++ b/data/Fable_46_Agricultural.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ev\Documents\Software Projects\SDSN GCH\ScenViz_Template\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EF31FAA-C3C5-4207-829C-1A3A55AFA7A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1108441-B068-48DC-A579-5A4FC3C4FB83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7F19FE23-2CEE-4DF1-B417-CD7D4A4FD5D6}"/>
   </bookViews>
@@ -501,11 +501,16 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="B1" sqref="B1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>